<commit_message>
Fixed a mistagged demolition derby as a race
</commit_message>
<xml_diff>
--- a/Wreckfest data.xlsx
+++ b/Wreckfest data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cce06eab74c9fcc4/Documents/Coding/Wreckfest Randomiser/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D08F4B45-C016-4594-BF00-9EEBA2D399FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{D08F4B45-C016-4594-BF00-9EEBA2D399FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{80E9AAF7-0B2A-4AC2-B1CF-CCDBD166351A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F60CAFD2-5075-47A9-A0F9-5239456A32B1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F60CAFD2-5075-47A9-A0F9-5239456A32B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Wreckfest data" sheetId="1" r:id="rId1"/>
@@ -2644,26 +2644,26 @@
   <dimension ref="A1:K115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.109375" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.28515625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="39.5703125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="8.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="39.5546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="8.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="27" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="28.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="8.85546875" style="3"/>
+    <col min="10" max="10" width="21.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.88671875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>629</v>
       </c>
@@ -2698,7 +2698,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -2733,7 +2733,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -2768,7 +2768,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -2803,7 +2803,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -2838,7 +2838,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -2849,7 +2849,7 @@
         <v>14</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>619</v>
+        <v>17</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>1</v>
@@ -2873,7 +2873,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -2908,7 +2908,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -2943,7 +2943,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -2978,7 +2978,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -3013,7 +3013,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -3048,7 +3048,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -3083,7 +3083,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -3118,7 +3118,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -3153,7 +3153,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -3188,7 +3188,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -3223,7 +3223,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -3258,7 +3258,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -3293,7 +3293,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -3328,7 +3328,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -3363,7 +3363,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -3398,7 +3398,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -3433,7 +3433,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -3468,7 +3468,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -3503,7 +3503,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -3538,7 +3538,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>25</v>
       </c>
@@ -3573,7 +3573,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>26</v>
       </c>
@@ -3608,7 +3608,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>27</v>
       </c>
@@ -3643,7 +3643,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>28</v>
       </c>
@@ -3678,7 +3678,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>29</v>
       </c>
@@ -3713,7 +3713,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -3748,7 +3748,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -3783,7 +3783,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -3818,7 +3818,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -3853,7 +3853,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>34</v>
       </c>
@@ -3888,7 +3888,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>35</v>
       </c>
@@ -3923,7 +3923,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>36</v>
       </c>
@@ -3958,7 +3958,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>37</v>
       </c>
@@ -3993,7 +3993,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>38</v>
       </c>
@@ -4028,7 +4028,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>39</v>
       </c>
@@ -4063,7 +4063,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>40</v>
       </c>
@@ -4098,7 +4098,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
         <v>41</v>
       </c>
@@ -4133,7 +4133,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <v>42</v>
       </c>
@@ -4168,7 +4168,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <v>43</v>
       </c>
@@ -4203,7 +4203,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <v>44</v>
       </c>
@@ -4238,7 +4238,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <v>45</v>
       </c>
@@ -4273,7 +4273,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
         <v>46</v>
       </c>
@@ -4308,7 +4308,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>47</v>
       </c>
@@ -4343,7 +4343,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
         <v>48</v>
       </c>
@@ -4378,7 +4378,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4">
         <v>49</v>
       </c>
@@ -4413,7 +4413,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4">
         <v>50</v>
       </c>
@@ -4448,7 +4448,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="4">
         <v>51</v>
       </c>
@@ -4483,7 +4483,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4">
         <v>52</v>
       </c>
@@ -4518,7 +4518,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="4">
         <v>53</v>
       </c>
@@ -4553,7 +4553,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="4">
         <v>54</v>
       </c>
@@ -4588,7 +4588,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="4">
         <v>55</v>
       </c>
@@ -4623,7 +4623,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="4">
         <v>56</v>
       </c>
@@ -4658,7 +4658,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="4">
         <v>57</v>
       </c>
@@ -4693,7 +4693,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="4">
         <v>58</v>
       </c>
@@ -4728,7 +4728,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="4">
         <v>59</v>
       </c>
@@ -4763,7 +4763,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="4">
         <v>60</v>
       </c>
@@ -4798,7 +4798,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="4">
         <v>61</v>
       </c>
@@ -4833,7 +4833,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4">
         <v>62</v>
       </c>
@@ -4868,7 +4868,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="4">
         <v>63</v>
       </c>
@@ -4903,7 +4903,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="65" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="4">
         <v>64</v>
       </c>
@@ -4938,7 +4938,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="66" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="4">
         <v>65</v>
       </c>
@@ -4973,7 +4973,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="67" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="4">
         <v>66</v>
       </c>
@@ -5008,7 +5008,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="68" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="4">
         <v>67</v>
       </c>
@@ -5043,7 +5043,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="69" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="4">
         <v>68</v>
       </c>
@@ -5078,7 +5078,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="70" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="4">
         <v>69</v>
       </c>
@@ -5113,7 +5113,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="71" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="4">
         <v>70</v>
       </c>
@@ -5148,7 +5148,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="72" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="4">
         <v>71</v>
       </c>
@@ -5183,7 +5183,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="73" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="4">
         <v>72</v>
       </c>
@@ -5218,7 +5218,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="74" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="4">
         <v>73</v>
       </c>
@@ -5253,7 +5253,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="75" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A75" s="4">
         <v>74</v>
       </c>
@@ -5288,7 +5288,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="76" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A76" s="4">
         <v>75</v>
       </c>
@@ -5323,7 +5323,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="77" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A77" s="4">
         <v>76</v>
       </c>
@@ -5358,7 +5358,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="78" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="4">
         <v>77</v>
       </c>
@@ -5393,7 +5393,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="79" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="4">
         <v>78</v>
       </c>
@@ -5428,7 +5428,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="80" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="4">
         <v>79</v>
       </c>
@@ -5463,7 +5463,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="81" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="4">
         <v>80</v>
       </c>
@@ -5498,7 +5498,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="82" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="4">
         <v>81</v>
       </c>
@@ -5533,7 +5533,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="83" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="4">
         <v>82</v>
       </c>
@@ -5568,7 +5568,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="84" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="4">
         <v>83</v>
       </c>
@@ -5603,7 +5603,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="85" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="4">
         <v>84</v>
       </c>
@@ -5638,7 +5638,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="86" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="4">
         <v>85</v>
       </c>
@@ -5673,7 +5673,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="87" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="4">
         <v>86</v>
       </c>
@@ -5708,7 +5708,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="88" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="4">
         <v>87</v>
       </c>
@@ -5743,7 +5743,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="89" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="4">
         <v>88</v>
       </c>
@@ -5778,7 +5778,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="4">
         <v>89</v>
       </c>
@@ -5813,7 +5813,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="91" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="4">
         <v>90</v>
       </c>
@@ -5848,7 +5848,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="92" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="4">
         <v>91</v>
       </c>
@@ -5883,7 +5883,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="93" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="4">
         <v>92</v>
       </c>
@@ -5918,7 +5918,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="94" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="4">
         <v>93</v>
       </c>
@@ -5953,7 +5953,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="95" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="4">
         <v>94</v>
       </c>
@@ -5988,7 +5988,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="96" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="4">
         <v>95</v>
       </c>
@@ -6023,7 +6023,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="97" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="4">
         <v>96</v>
       </c>
@@ -6058,7 +6058,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="98" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="4">
         <v>97</v>
       </c>
@@ -6093,7 +6093,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="99" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="4">
         <v>98</v>
       </c>
@@ -6128,7 +6128,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="100" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="4">
         <v>99</v>
       </c>
@@ -6163,7 +6163,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="101" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="4">
         <v>100</v>
       </c>
@@ -6198,7 +6198,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="102" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="4">
         <v>101</v>
       </c>
@@ -6233,7 +6233,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="103" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="4">
         <v>102</v>
       </c>
@@ -6268,7 +6268,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="104" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="4">
         <v>103</v>
       </c>
@@ -6303,7 +6303,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="105" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="4">
         <v>104</v>
       </c>
@@ -6338,7 +6338,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="106" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="4">
         <v>105</v>
       </c>
@@ -6373,7 +6373,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="107" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="4">
         <v>106</v>
       </c>
@@ -6408,7 +6408,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="108" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="4">
         <v>107</v>
       </c>
@@ -6443,7 +6443,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="109" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="4">
         <v>108</v>
       </c>
@@ -6478,7 +6478,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="110" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="4">
         <v>109</v>
       </c>
@@ -6513,7 +6513,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="111" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="4">
         <v>110</v>
       </c>
@@ -6548,7 +6548,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="112" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="4">
         <v>111</v>
       </c>
@@ -6583,7 +6583,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="113" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="4">
         <v>112</v>
       </c>
@@ -6618,7 +6618,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="114" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="4">
         <v>113</v>
       </c>
@@ -6653,7 +6653,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="115" spans="1:11" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:11" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="4">
         <v>114</v>
       </c>
@@ -6703,28 +6703,28 @@
       <selection activeCell="N34" sqref="N1:N1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.7109375" style="7" customWidth="1"/>
+    <col min="1" max="1" width="8.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.6640625" style="7" customWidth="1"/>
     <col min="3" max="3" width="41" style="7" customWidth="1"/>
-    <col min="4" max="4" width="20.85546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" style="7" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="33.7109375" style="7" customWidth="1"/>
-    <col min="14" max="16" width="8.85546875" style="7"/>
-    <col min="17" max="17" width="28.140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="33.6640625" style="7" customWidth="1"/>
+    <col min="14" max="16" width="8.88671875" style="7"/>
+    <col min="17" max="17" width="28.109375" style="7" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="20" style="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="8.85546875" style="7"/>
+    <col min="19" max="16384" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
         <v>629</v>
       </c>
@@ -6765,7 +6765,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="12">
         <v>1</v>
       </c>
@@ -6806,7 +6806,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12">
         <v>2</v>
       </c>
@@ -6847,7 +6847,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="12">
         <v>3</v>
       </c>
@@ -6888,7 +6888,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="12">
         <v>4</v>
       </c>
@@ -6929,7 +6929,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="12">
         <v>5</v>
       </c>
@@ -6970,7 +6970,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="12">
         <v>6</v>
       </c>
@@ -7011,7 +7011,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="12">
         <v>7</v>
       </c>
@@ -7052,7 +7052,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="12">
         <v>8</v>
       </c>
@@ -7093,7 +7093,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12">
         <v>9</v>
       </c>
@@ -7134,7 +7134,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="12">
         <v>10</v>
       </c>
@@ -7175,7 +7175,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="12">
         <v>11</v>
       </c>
@@ -7216,7 +7216,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="12">
         <v>12</v>
       </c>
@@ -7257,7 +7257,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="12">
         <v>13</v>
       </c>
@@ -7298,7 +7298,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>14</v>
       </c>
@@ -7339,7 +7339,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
         <v>15</v>
       </c>
@@ -7380,7 +7380,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
         <v>16</v>
       </c>
@@ -7421,7 +7421,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="12">
         <v>17</v>
       </c>
@@ -7462,7 +7462,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="12">
         <v>18</v>
       </c>
@@ -7503,7 +7503,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
         <v>19</v>
       </c>
@@ -7544,7 +7544,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="12">
         <v>20</v>
       </c>
@@ -7585,7 +7585,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="12">
         <v>21</v>
       </c>
@@ -7626,7 +7626,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="12">
         <v>22</v>
       </c>
@@ -7667,7 +7667,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="12">
         <v>23</v>
       </c>
@@ -7708,7 +7708,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="12">
         <v>24</v>
       </c>
@@ -7749,7 +7749,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="12">
         <v>25</v>
       </c>
@@ -7790,7 +7790,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="12">
         <v>26</v>
       </c>
@@ -7831,7 +7831,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="12">
         <v>27</v>
       </c>
@@ -7872,7 +7872,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="12">
         <v>28</v>
       </c>
@@ -7913,7 +7913,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="12">
         <v>29</v>
       </c>
@@ -7954,7 +7954,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="12">
         <v>30</v>
       </c>
@@ -7995,7 +7995,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="12">
         <v>31</v>
       </c>
@@ -8036,7 +8036,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="12">
         <v>32</v>
       </c>
@@ -8077,7 +8077,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="12">
         <v>33</v>
       </c>
@@ -8118,7 +8118,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="12">
         <v>34</v>
       </c>
@@ -8159,7 +8159,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="12">
         <v>35</v>
       </c>
@@ -8200,7 +8200,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="12">
         <v>36</v>
       </c>
@@ -8241,7 +8241,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="12">
         <v>37</v>
       </c>
@@ -8282,7 +8282,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="12">
         <v>38</v>
       </c>
@@ -8323,7 +8323,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="12">
         <v>39</v>
       </c>
@@ -8364,7 +8364,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="12">
         <v>40</v>
       </c>
@@ -8405,7 +8405,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="12">
         <v>41</v>
       </c>
@@ -8446,7 +8446,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="12">
         <v>42</v>
       </c>
@@ -8487,7 +8487,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="12">
         <v>43</v>
       </c>
@@ -8528,7 +8528,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="12">
         <v>44</v>
       </c>
@@ -8569,7 +8569,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="12">
         <v>45</v>
       </c>
@@ -8610,7 +8610,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="12">
         <v>46</v>
       </c>
@@ -8651,7 +8651,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="48" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="12">
         <v>47</v>
       </c>
@@ -8692,7 +8692,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="49" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="12">
         <v>48</v>
       </c>
@@ -8733,7 +8733,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="50" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="12">
         <v>49</v>
       </c>
@@ -8774,7 +8774,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="51" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="12">
         <v>50</v>
       </c>
@@ -8815,7 +8815,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="52" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="12">
         <v>51</v>
       </c>
@@ -8856,7 +8856,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="53" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="12">
         <v>52</v>
       </c>
@@ -8897,7 +8897,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="54" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="12">
         <v>53</v>
       </c>
@@ -8938,7 +8938,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="55" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="12">
         <v>54</v>
       </c>
@@ -8979,7 +8979,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="56" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="12">
         <v>55</v>
       </c>
@@ -9020,7 +9020,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="57" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="12">
         <v>56</v>
       </c>
@@ -9061,7 +9061,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="58" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="12">
         <v>57</v>
       </c>
@@ -9102,7 +9102,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="59" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="12">
         <v>58</v>
       </c>
@@ -9143,7 +9143,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="60" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="12">
         <v>59</v>
       </c>
@@ -9184,7 +9184,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="61" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="12">
         <v>60</v>
       </c>
@@ -9225,7 +9225,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="62" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="12">
         <v>61</v>
       </c>
@@ -9266,7 +9266,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="63" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="12">
         <v>62</v>
       </c>
@@ -9307,7 +9307,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="64" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A64" s="12">
         <v>63</v>
       </c>
@@ -9348,7 +9348,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="65" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="12">
         <v>64</v>
       </c>
@@ -9389,7 +9389,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="66" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="12">
         <v>65</v>
       </c>

</xml_diff>